<commit_message>
Correccion en WHILE y REPEAT
Se corrige el salto incondicional del WHILE y se elimina el REPEAT que no lo piden
</commit_message>
<xml_diff>
--- a/Segunda_entrega_correccion/CORRECCIONES SEGUNDA ENTREGA.xlsx
+++ b/Segunda_entrega_correccion/CORRECCIONES SEGUNDA ENTREGA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="82">
   <si>
     <t>LEXICO</t>
   </si>
@@ -248,18 +248,6 @@
     <t xml:space="preserve"> Errores</t>
   </si>
   <si>
-    <t>Aprobado por el profesor</t>
-  </si>
-  <si>
-    <t>Corregido por nosotros</t>
-  </si>
-  <si>
-    <t>Aprobado con observacion por el profesor</t>
-  </si>
-  <si>
-    <t>Desprobado por profesor</t>
-  </si>
-  <si>
     <t>Funciona solo con asignaciones que tienen en el lado derecho, una cte o id. Si se coloca una expresión en el lado derecho, no funciona:
 a = b = c = 5 +8. Aplicar resolución vista en clase.</t>
   </si>
@@ -277,6 +265,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ARREGLADO</t>
   </si>
 </sst>
 </file>
@@ -294,30 +285,36 @@
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -372,7 +369,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,20 +424,8 @@
         <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF70AD47"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -544,31 +529,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -604,59 +569,91 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -673,71 +670,17 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1043,35 +986,35 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="69.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="58.140625" style="62" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.140625" style="29" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1089,10 +1032,10 @@
       </c>
       <c r="G2" s="8">
         <f>COUNTIF(B:B,"NO")</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
@@ -1102,7 +1045,7 @@
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
@@ -1111,15 +1054,8 @@
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
-      <c r="F4" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="19" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
@@ -1128,15 +1064,8 @@
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
-      <c r="F5" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>8</v>
       </c>
@@ -1145,15 +1074,8 @@
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
-      <c r="F6" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
@@ -1162,15 +1084,8 @@
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
-      <c r="F7" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="37"/>
-      <c r="H7" s="19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>10</v>
       </c>
@@ -1180,21 +1095,21 @@
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>5</v>
+      <c r="B9" s="61" t="s">
+        <v>81</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>14</v>
       </c>
@@ -1204,7 +1119,7 @@
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>15</v>
       </c>
@@ -1214,7 +1129,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>16</v>
       </c>
@@ -1224,7 +1139,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>17</v>
       </c>
@@ -1234,7 +1149,7 @@
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>18</v>
       </c>
@@ -1244,15 +1159,15 @@
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
     </row>
-    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="46" t="s">
+    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>1</v>
       </c>
@@ -1313,16 +1228,16 @@
       <c r="B21" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="52"/>
+      <c r="C21" s="21"/>
       <c r="D21" s="14"/>
     </row>
     <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="47" t="s">
+      <c r="A22" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="43"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
@@ -1331,7 +1246,7 @@
       <c r="B23" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="53" t="s">
+      <c r="C23" s="22" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="9"/>
@@ -1343,7 +1258,7 @@
       <c r="B24" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="54"/>
+      <c r="C24" s="23"/>
       <c r="D24" s="13"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1353,7 +1268,7 @@
       <c r="B25" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="54"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="13"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1363,7 +1278,7 @@
       <c r="B26" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="54"/>
+      <c r="C26" s="23"/>
       <c r="D26" s="13"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1373,7 +1288,7 @@
       <c r="B27" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="54"/>
+      <c r="C27" s="23"/>
       <c r="D27" s="13"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1383,7 +1298,7 @@
       <c r="B28" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="54"/>
+      <c r="C28" s="23"/>
       <c r="D28" s="13"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1393,7 +1308,7 @@
       <c r="B29" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="54"/>
+      <c r="C29" s="23"/>
       <c r="D29" s="13"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1403,7 +1318,7 @@
       <c r="B30" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="54"/>
+      <c r="C30" s="23"/>
       <c r="D30" s="13"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1413,7 +1328,7 @@
       <c r="B31" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="54"/>
+      <c r="C31" s="23"/>
       <c r="D31" s="13"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1423,7 +1338,7 @@
       <c r="B32" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="54"/>
+      <c r="C32" s="23"/>
       <c r="D32" s="13"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1433,7 +1348,7 @@
       <c r="B33" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="54"/>
+      <c r="C33" s="23"/>
       <c r="D33" s="13"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1443,7 +1358,7 @@
       <c r="B34" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="54"/>
+      <c r="C34" s="23"/>
       <c r="D34" s="13"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1453,21 +1368,21 @@
       <c r="B35" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="54"/>
+      <c r="C35" s="23"/>
       <c r="D35" s="13"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="55" t="s">
+      <c r="B36" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="24" t="s">
         <v>41</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1477,29 +1392,29 @@
       <c r="B37" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="54"/>
+      <c r="C37" s="23"/>
       <c r="D37" s="13"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="54" t="s">
+      <c r="B38" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="23" t="s">
         <v>44</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A39" s="46" t="s">
+      <c r="A39" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="46"/>
-      <c r="C39" s="51"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="53"/>
       <c r="D39" s="14"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1509,7 +1424,7 @@
       <c r="B40" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C40" s="53" t="s">
+      <c r="C40" s="22" t="s">
         <v>3</v>
       </c>
       <c r="D40" s="9"/>
@@ -1521,17 +1436,17 @@
       <c r="B41" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="54"/>
+      <c r="C41" s="23"/>
       <c r="D41" s="13"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="54"/>
+      <c r="C42" s="23"/>
       <c r="D42" s="13"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1541,15 +1456,15 @@
       <c r="B43" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="56"/>
+      <c r="C43" s="25"/>
       <c r="D43" s="14"/>
     </row>
     <row r="44" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="38"/>
-      <c r="C44" s="39"/>
+      <c r="B44" s="54"/>
+      <c r="C44" s="55"/>
       <c r="D44" s="14"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1559,7 +1474,7 @@
       <c r="B45" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C45" s="57" t="s">
+      <c r="C45" s="26" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="9"/>
@@ -1568,32 +1483,32 @@
       <c r="A46" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="54"/>
+      <c r="B46" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="23"/>
       <c r="D46" s="11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="54"/>
+      <c r="C47" s="23"/>
       <c r="D47" s="13"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="54"/>
+      <c r="C48" s="23"/>
       <c r="D48" s="11"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1603,9 +1518,9 @@
       <c r="B49" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="54"/>
+      <c r="C49" s="23"/>
       <c r="D49" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1615,7 +1530,7 @@
       <c r="B50" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="54" t="s">
+      <c r="C50" s="23" t="s">
         <v>55</v>
       </c>
       <c r="D50" s="13"/>
@@ -1624,11 +1539,13 @@
       <c r="A51" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" s="54"/>
-      <c r="D51" s="13"/>
+      <c r="B51" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" s="23"/>
+      <c r="D51" s="11" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
@@ -1637,26 +1554,26 @@
       <c r="B52" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="54"/>
+      <c r="C52" s="23"/>
       <c r="D52" s="13"/>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="44" t="s">
+      <c r="A53" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="58" t="s">
+      <c r="B53" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="24"/>
+      <c r="D53" s="39"/>
     </row>
     <row r="54" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="45"/>
-      <c r="B54" s="41"/>
-      <c r="C54" s="59"/>
-      <c r="D54" s="26"/>
+      <c r="A54" s="32"/>
+      <c r="B54" s="57"/>
+      <c r="C54" s="52"/>
+      <c r="D54" s="35"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
@@ -1665,20 +1582,22 @@
       <c r="B55" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="56"/>
+      <c r="C55" s="25"/>
       <c r="D55" s="14"/>
     </row>
     <row r="56" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B56" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C56" s="60" t="s">
+      <c r="B56" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D56" s="13"/>
+      <c r="D56" s="63" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
@@ -1687,7 +1606,7 @@
       <c r="B57" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="54" t="s">
+      <c r="C57" s="23" t="s">
         <v>64</v>
       </c>
       <c r="D57" s="13"/>
@@ -1699,106 +1618,106 @@
       <c r="B58" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C58" s="61"/>
-      <c r="D58" s="21"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="20"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B59" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="68" t="s">
+      <c r="B59" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="D59" s="71" t="s">
-        <v>82</v>
+      <c r="D59" s="33" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="45"/>
-      <c r="B60" s="41"/>
-      <c r="C60" s="69"/>
-      <c r="D60" s="25"/>
+      <c r="A60" s="32"/>
+      <c r="B60" s="57"/>
+      <c r="C60" s="48"/>
+      <c r="D60" s="34"/>
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="45"/>
-      <c r="B61" s="41"/>
-      <c r="C61" s="69"/>
-      <c r="D61" s="25"/>
+      <c r="A61" s="32"/>
+      <c r="B61" s="57"/>
+      <c r="C61" s="48"/>
+      <c r="D61" s="34"/>
     </row>
     <row r="62" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="45"/>
-      <c r="B62" s="41"/>
-      <c r="C62" s="70"/>
-      <c r="D62" s="26"/>
+      <c r="A62" s="32"/>
+      <c r="B62" s="57"/>
+      <c r="C62" s="49"/>
+      <c r="D62" s="35"/>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="44" t="s">
+      <c r="A63" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="43" t="s">
+      <c r="B63" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C63" s="63" t="s">
-        <v>79</v>
-      </c>
-      <c r="D63" s="27"/>
+      <c r="C63" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="D63" s="36"/>
     </row>
     <row r="64" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="45"/>
-      <c r="B64" s="41"/>
-      <c r="C64" s="64"/>
-      <c r="D64" s="28"/>
+      <c r="A64" s="32"/>
+      <c r="B64" s="57"/>
+      <c r="C64" s="45"/>
+      <c r="D64" s="37"/>
     </row>
     <row r="65" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A65" s="45"/>
-      <c r="B65" s="41"/>
-      <c r="C65" s="64"/>
-      <c r="D65" s="28"/>
+      <c r="A65" s="32"/>
+      <c r="B65" s="57"/>
+      <c r="C65" s="45"/>
+      <c r="D65" s="37"/>
     </row>
     <row r="66" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="45"/>
-      <c r="B66" s="41"/>
-      <c r="C66" s="65"/>
-      <c r="D66" s="29"/>
+      <c r="A66" s="32"/>
+      <c r="B66" s="57"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="38"/>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="44" t="s">
+      <c r="A67" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="B67" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C67" s="63" t="s">
+      <c r="B67" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="D67" s="27"/>
+      <c r="D67" s="36"/>
     </row>
     <row r="68" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A68" s="45"/>
-      <c r="B68" s="67"/>
-      <c r="C68" s="64"/>
-      <c r="D68" s="28"/>
+      <c r="A68" s="32"/>
+      <c r="B68" s="60"/>
+      <c r="C68" s="45"/>
+      <c r="D68" s="37"/>
     </row>
     <row r="69" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="45"/>
-      <c r="B69" s="67"/>
-      <c r="C69" s="64"/>
-      <c r="D69" s="28"/>
+      <c r="A69" s="32"/>
+      <c r="B69" s="60"/>
+      <c r="C69" s="45"/>
+      <c r="D69" s="37"/>
     </row>
     <row r="70" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A70" s="45"/>
-      <c r="B70" s="67"/>
-      <c r="C70" s="64"/>
-      <c r="D70" s="28"/>
+      <c r="A70" s="32"/>
+      <c r="B70" s="60"/>
+      <c r="C70" s="45"/>
+      <c r="D70" s="37"/>
     </row>
     <row r="71" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="45"/>
-      <c r="B71" s="67"/>
-      <c r="C71" s="65"/>
-      <c r="D71" s="29"/>
+      <c r="A71" s="32"/>
+      <c r="B71" s="60"/>
+      <c r="C71" s="46"/>
+      <c r="D71" s="38"/>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
@@ -1807,7 +1726,7 @@
       <c r="B72" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C72" s="66" t="s">
+      <c r="C72" s="30" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1815,7 +1734,7 @@
       <c r="D74" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="21">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A22:D22"/>
@@ -1837,10 +1756,6 @@
     <mergeCell ref="D67:D71"/>
     <mergeCell ref="D63:D66"/>
     <mergeCell ref="D53:D54"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Between y No Between en While y Asignacion
</commit_message>
<xml_diff>
--- a/Segunda_entrega_correccion/CORRECCIONES SEGUNDA ENTREGA.xlsx
+++ b/Segunda_entrega_correccion/CORRECCIONES SEGUNDA ENTREGA.xlsx
@@ -1,20 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Compilador\Compilador\Segunda_entrega_correccion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280E4839-5425-4B14-9E92-7CAB9517FEF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="585" windowWidth="19815" windowHeight="6090"/>
+    <workbookView xWindow="270" yWindow="585" windowWidth="19815" windowHeight="6090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="86">
   <si>
     <t>LEXICO</t>
   </si>
@@ -268,11 +281,23 @@
   <si>
     <t>[Mauro] - Se hizo asi porque funciona mejor para AND y OR y evitar harcodear tanto.</t>
   </si>
+  <si>
+    <t>[Sandro] - Se resta -2 al result de strlen</t>
+  </si>
+  <si>
+    <t>[Leandro] - Corregido</t>
+  </si>
+  <si>
+    <t>[Anonimo] - Corregido</t>
+  </si>
+  <si>
+    <t>[Leandro] - Si coloco el between del lado derecho de una asignacion funciona. En el if el between devuelve 1 o 0, y lo comparo con 1, y en el not between con 0. Igual con el while.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -532,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -565,9 +590,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -599,6 +621,34 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -632,14 +682,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -657,32 +703,24 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,12 +732,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -741,7 +782,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -774,9 +815,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -809,6 +867,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -984,21 +1059,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63:D66"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67:C71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="69.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.140625" style="29" customWidth="1"/>
+    <col min="3" max="3" width="58.140625" style="28" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
@@ -1006,12 +1081,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1034,7 +1109,7 @@
       </c>
       <c r="G2" s="8">
         <f>COUNTIF(B:B,"NO")</f>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1101,7 +1176,7 @@
       <c r="A9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>79</v>
       </c>
       <c r="C9" s="12" t="s">
@@ -1162,12 +1237,12 @@
       <c r="D14" s="12"/>
     </row>
     <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
@@ -1215,13 +1290,15 @@
       <c r="A20" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="18" t="s">
-        <v>5</v>
+      <c r="B20" s="30" t="s">
+        <v>79</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="13"/>
+      <c r="D20" s="13" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
@@ -1230,16 +1307,16 @@
       <c r="B21" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="21"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="14"/>
     </row>
     <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="37"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="46"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
@@ -1248,7 +1325,7 @@
       <c r="B23" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="9"/>
@@ -1260,7 +1337,7 @@
       <c r="B24" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="23"/>
+      <c r="C24" s="22"/>
       <c r="D24" s="13"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1270,7 +1347,7 @@
       <c r="B25" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="23"/>
+      <c r="C25" s="22"/>
       <c r="D25" s="13"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1280,7 +1357,7 @@
       <c r="B26" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="23"/>
+      <c r="C26" s="22"/>
       <c r="D26" s="13"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1290,7 +1367,7 @@
       <c r="B27" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="23"/>
+      <c r="C27" s="22"/>
       <c r="D27" s="13"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1300,7 +1377,7 @@
       <c r="B28" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="23"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="13"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1310,7 +1387,7 @@
       <c r="B29" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="23"/>
+      <c r="C29" s="22"/>
       <c r="D29" s="13"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1320,7 +1397,7 @@
       <c r="B30" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="23"/>
+      <c r="C30" s="22"/>
       <c r="D30" s="13"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1330,7 +1407,7 @@
       <c r="B31" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="23"/>
+      <c r="C31" s="22"/>
       <c r="D31" s="13"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1340,7 +1417,7 @@
       <c r="B32" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="23"/>
+      <c r="C32" s="22"/>
       <c r="D32" s="13"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1350,7 +1427,7 @@
       <c r="B33" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="23"/>
+      <c r="C33" s="22"/>
       <c r="D33" s="13"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1360,7 +1437,7 @@
       <c r="B34" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="23"/>
+      <c r="C34" s="22"/>
       <c r="D34" s="13"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1370,17 +1447,17 @@
       <c r="B35" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="23"/>
+      <c r="C35" s="22"/>
       <c r="D35" s="13"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="23" t="s">
         <v>41</v>
       </c>
       <c r="D36" s="11" t="s">
@@ -1394,17 +1471,17 @@
       <c r="B37" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="23"/>
+      <c r="C37" s="22"/>
       <c r="D37" s="13"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="C38" s="22" t="s">
         <v>44</v>
       </c>
       <c r="D38" s="11" t="s">
@@ -1412,11 +1489,11 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A39" s="34" t="s">
+      <c r="A39" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="34"/>
-      <c r="C39" s="49"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="56"/>
       <c r="D39" s="14"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1426,7 +1503,7 @@
       <c r="B40" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D40" s="9"/>
@@ -1438,18 +1515,20 @@
       <c r="B41" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="23"/>
+      <c r="C41" s="22"/>
       <c r="D41" s="13"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="13"/>
+      <c r="B42" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="22"/>
+      <c r="D42" s="13" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
@@ -1458,15 +1537,15 @@
       <c r="B43" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="25"/>
+      <c r="C43" s="24"/>
       <c r="D43" s="14"/>
     </row>
     <row r="44" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A44" s="50" t="s">
+      <c r="A44" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="50"/>
-      <c r="C44" s="51"/>
+      <c r="B44" s="57"/>
+      <c r="C44" s="58"/>
       <c r="D44" s="14"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1476,7 +1555,7 @@
       <c r="B45" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C45" s="26" t="s">
+      <c r="C45" s="25" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="9"/>
@@ -1485,10 +1564,10 @@
       <c r="A46" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="31" t="s">
+      <c r="B46" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="23"/>
+      <c r="C46" s="22"/>
       <c r="D46" s="11" t="s">
         <v>75</v>
       </c>
@@ -1497,20 +1576,20 @@
       <c r="A47" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="19" t="s">
+      <c r="B47" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="23"/>
+      <c r="C47" s="22"/>
       <c r="D47" s="13"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="19" t="s">
+      <c r="B48" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="23"/>
+      <c r="C48" s="22"/>
       <c r="D48" s="11"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1520,7 +1599,7 @@
       <c r="B49" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="23"/>
+      <c r="C49" s="22"/>
       <c r="D49" s="11" t="s">
         <v>78</v>
       </c>
@@ -1529,22 +1608,24 @@
       <c r="A50" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="23" t="s">
+      <c r="B50" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="D50" s="13"/>
+      <c r="D50" s="13" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="31" t="s">
+      <c r="B51" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C51" s="23"/>
+      <c r="C51" s="22"/>
       <c r="D51" s="11" t="s">
         <v>75</v>
       </c>
@@ -1556,26 +1637,26 @@
       <c r="B52" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="23"/>
+      <c r="C52" s="22"/>
       <c r="D52" s="13"/>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="48" t="s">
+      <c r="A53" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="46" t="s">
+      <c r="B53" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="61"/>
+      <c r="D53" s="41"/>
     </row>
     <row r="54" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="45"/>
-      <c r="B54" s="53"/>
-      <c r="C54" s="47"/>
-      <c r="D54" s="57"/>
+      <c r="A54" s="34"/>
+      <c r="B54" s="60"/>
+      <c r="C54" s="55"/>
+      <c r="D54" s="42"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
@@ -1584,20 +1665,20 @@
       <c r="B55" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="25"/>
+      <c r="C55" s="24"/>
       <c r="D55" s="14"/>
     </row>
     <row r="56" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B56" s="32" t="s">
+      <c r="B56" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="C56" s="27" t="s">
+      <c r="C56" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="D56" s="33" t="s">
+      <c r="D56" s="32" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1608,7 +1689,7 @@
       <c r="B57" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="23" t="s">
+      <c r="C57" s="22" t="s">
         <v>64</v>
       </c>
       <c r="D57" s="13"/>
@@ -1620,106 +1701,108 @@
       <c r="B58" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C58" s="28"/>
-      <c r="D58" s="20"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="19"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="44" t="s">
+      <c r="A59" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="B59" s="54" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="41" t="s">
+      <c r="B59" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="D59" s="64" t="s">
+      <c r="D59" s="35" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="45"/>
-      <c r="B60" s="53"/>
-      <c r="C60" s="42"/>
-      <c r="D60" s="62"/>
+      <c r="A60" s="34"/>
+      <c r="B60" s="60"/>
+      <c r="C60" s="51"/>
+      <c r="D60" s="36"/>
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="45"/>
-      <c r="B61" s="53"/>
-      <c r="C61" s="42"/>
-      <c r="D61" s="62"/>
+      <c r="A61" s="34"/>
+      <c r="B61" s="60"/>
+      <c r="C61" s="51"/>
+      <c r="D61" s="36"/>
     </row>
     <row r="62" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="45"/>
-      <c r="B62" s="53"/>
-      <c r="C62" s="43"/>
-      <c r="D62" s="63"/>
+      <c r="A62" s="34"/>
+      <c r="B62" s="60"/>
+      <c r="C62" s="52"/>
+      <c r="D62" s="37"/>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="48" t="s">
+      <c r="A63" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="55" t="s">
+      <c r="B63" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="C63" s="38" t="s">
+      <c r="C63" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="D63" s="58"/>
+      <c r="D63" s="38"/>
     </row>
     <row r="64" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="45"/>
-      <c r="B64" s="53"/>
-      <c r="C64" s="39"/>
-      <c r="D64" s="59"/>
+      <c r="A64" s="34"/>
+      <c r="B64" s="60"/>
+      <c r="C64" s="48"/>
+      <c r="D64" s="39"/>
     </row>
     <row r="65" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A65" s="45"/>
-      <c r="B65" s="53"/>
-      <c r="C65" s="39"/>
-      <c r="D65" s="59"/>
+      <c r="A65" s="34"/>
+      <c r="B65" s="60"/>
+      <c r="C65" s="48"/>
+      <c r="D65" s="39"/>
     </row>
     <row r="66" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="45"/>
-      <c r="B66" s="53"/>
-      <c r="C66" s="40"/>
-      <c r="D66" s="60"/>
+      <c r="A66" s="34"/>
+      <c r="B66" s="60"/>
+      <c r="C66" s="49"/>
+      <c r="D66" s="40"/>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="48" t="s">
+      <c r="A67" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="B67" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="C67" s="38" t="s">
+      <c r="B67" s="67" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="D67" s="58"/>
-    </row>
-    <row r="68" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A68" s="45"/>
-      <c r="B68" s="56"/>
-      <c r="C68" s="39"/>
-      <c r="D68" s="59"/>
-    </row>
-    <row r="69" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="45"/>
-      <c r="B69" s="56"/>
-      <c r="C69" s="39"/>
-      <c r="D69" s="59"/>
-    </row>
-    <row r="70" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A70" s="45"/>
-      <c r="B70" s="56"/>
-      <c r="C70" s="39"/>
-      <c r="D70" s="59"/>
+      <c r="D67" s="64" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="34"/>
+      <c r="B68" s="68"/>
+      <c r="C68" s="48"/>
+      <c r="D68" s="65"/>
+    </row>
+    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="34"/>
+      <c r="B69" s="68"/>
+      <c r="C69" s="48"/>
+      <c r="D69" s="65"/>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="34"/>
+      <c r="B70" s="68"/>
+      <c r="C70" s="48"/>
+      <c r="D70" s="65"/>
     </row>
     <row r="71" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="45"/>
-      <c r="B71" s="56"/>
-      <c r="C71" s="40"/>
-      <c r="D71" s="60"/>
+      <c r="A71" s="34"/>
+      <c r="B71" s="69"/>
+      <c r="C71" s="49"/>
+      <c r="D71" s="66"/>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
@@ -1728,7 +1811,7 @@
       <c r="B72" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C72" s="30" t="s">
+      <c r="C72" s="29" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1737,11 +1820,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="D59:D62"/>
-    <mergeCell ref="D67:D71"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="D53:D54"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A22:D22"/>
@@ -1758,6 +1836,11 @@
     <mergeCell ref="B59:B62"/>
     <mergeCell ref="B63:B66"/>
     <mergeCell ref="B67:B71"/>
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="D59:D62"/>
+    <mergeCell ref="D67:D71"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="D53:D54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Ver de corregir comparacion en if between y while btn
</commit_message>
<xml_diff>
--- a/Segunda_entrega_correccion/CORRECCIONES SEGUNDA ENTREGA.xlsx
+++ b/Segunda_entrega_correccion/CORRECCIONES SEGUNDA ENTREGA.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Compilador\Compilador\Segunda_entrega_correccion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280E4839-5425-4B14-9E92-7CAB9517FEF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="585" windowWidth="19815" windowHeight="6090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="270" yWindow="585" windowWidth="19815" windowHeight="6090"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="87">
   <si>
     <t>LEXICO</t>
   </si>
@@ -293,12 +287,15 @@
   <si>
     <t>[Leandro] - Si coloco el between del lado derecho de una asignacion funciona. En el if el between devuelve 1 o 0, y lo comparo con 1, y en el not between con 0. Igual con el while.</t>
   </si>
+  <si>
+    <t>[Mauro] - Ahora tolera expresiones</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -392,8 +389,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,6 +451,12 @@
         <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -557,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -566,7 +575,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -611,7 +619,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -621,71 +628,48 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -700,10 +684,24 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -713,14 +711,32 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -740,7 +756,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -782,7 +798,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -815,26 +831,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -867,23 +866,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1059,21 +1041,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67:C71"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="69.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.140625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.140625" style="27" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
@@ -1081,472 +1063,472 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <f>COUNTIF(B:B,"NO")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
+      <c r="B3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
+      <c r="B4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
+      <c r="B5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
+      <c r="B6" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
+      <c r="B8" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
+      <c r="B11" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
+      <c r="B12" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
+      <c r="B13" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+      <c r="B14" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="9"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="13"/>
+      <c r="B17" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="12"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="13"/>
+      <c r="B18" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="12"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="13"/>
+      <c r="B19" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="12"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="12" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="14"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="13"/>
     </row>
     <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="46"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="35"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="9"/>
+      <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="13"/>
+      <c r="B24" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="21"/>
+      <c r="D24" s="12"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="13"/>
+      <c r="B25" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="21"/>
+      <c r="D25" s="12"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="13"/>
+      <c r="B26" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="21"/>
+      <c r="D26" s="12"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="13"/>
+      <c r="B27" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="21"/>
+      <c r="D27" s="12"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="13"/>
+      <c r="B28" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="21"/>
+      <c r="D28" s="12"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="13"/>
+      <c r="B29" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="21"/>
+      <c r="D29" s="12"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="13"/>
+      <c r="B30" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="21"/>
+      <c r="D30" s="12"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="13"/>
+      <c r="B31" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="21"/>
+      <c r="D31" s="12"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="13"/>
+      <c r="B32" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="21"/>
+      <c r="D32" s="12"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="13"/>
+      <c r="B33" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="21"/>
+      <c r="D33" s="12"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="13"/>
+      <c r="B34" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="21"/>
+      <c r="D34" s="12"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="13"/>
+      <c r="B35" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="21"/>
+      <c r="D35" s="12"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="22"/>
-      <c r="D37" s="13"/>
+      <c r="B37" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="21"/>
+      <c r="D37" s="12"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A39" s="43" t="s">
+      <c r="A39" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="43"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="14"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="13"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="C40" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D40" s="9"/>
+      <c r="D40" s="8"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="13"/>
+      <c r="B41" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="21"/>
+      <c r="D41" s="12"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="13" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="12" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="14"/>
+      <c r="B43" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="23"/>
+      <c r="D43" s="13"/>
     </row>
     <row r="44" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A44" s="57" t="s">
+      <c r="A44" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="57"/>
-      <c r="C44" s="58"/>
-      <c r="D44" s="14"/>
+      <c r="B44" s="48"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="13"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
@@ -1555,271 +1537,278 @@
       <c r="B45" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C45" s="25" t="s">
+      <c r="C45" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D45" s="9"/>
+      <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="22"/>
-      <c r="D46" s="11" t="s">
+      <c r="C46" s="21"/>
+      <c r="D46" s="10" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="22"/>
-      <c r="D47" s="13"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="12"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
+      <c r="A48" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="22"/>
-      <c r="D48" s="11"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="10"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="22"/>
-      <c r="D49" s="11" t="s">
+      <c r="B49" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="21"/>
+      <c r="D49" s="10" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="30" t="s">
+      <c r="B50" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C50" s="63" t="s">
+      <c r="C50" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D50" s="12" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="30" t="s">
+      <c r="B51" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C51" s="22"/>
-      <c r="D51" s="11" t="s">
+      <c r="C51" s="21"/>
+      <c r="D51" s="10" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="22"/>
-      <c r="D52" s="13"/>
+      <c r="B52" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="21"/>
+      <c r="D52" s="12"/>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="33" t="s">
+      <c r="A53" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="54" t="s">
+      <c r="B53" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="41"/>
+      <c r="D53" s="62"/>
     </row>
     <row r="54" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="34"/>
-      <c r="B54" s="60"/>
-      <c r="C54" s="55"/>
-      <c r="D54" s="42"/>
+      <c r="A54" s="43"/>
+      <c r="B54" s="51"/>
+      <c r="C54" s="45"/>
+      <c r="D54" s="63"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B55" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" s="24"/>
-      <c r="D55" s="14"/>
+      <c r="B55" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="23"/>
+      <c r="D55" s="13"/>
     </row>
     <row r="56" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B56" s="31" t="s">
+      <c r="B56" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C56" s="26" t="s">
+      <c r="C56" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D56" s="32" t="s">
+      <c r="D56" s="30" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="22" t="s">
+      <c r="C57" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="D57" s="13"/>
+      <c r="D57" s="12"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
+      <c r="A58" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B58" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="27"/>
-      <c r="D58" s="19"/>
+      <c r="B58" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="26"/>
+      <c r="D58" s="18"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="53" t="s">
+      <c r="A59" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="B59" s="61" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="50" t="s">
+      <c r="B59" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="D59" s="35" t="s">
+      <c r="D59" s="56" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="34"/>
-      <c r="B60" s="60"/>
-      <c r="C60" s="51"/>
-      <c r="D60" s="36"/>
+      <c r="A60" s="43"/>
+      <c r="B60" s="51"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="57"/>
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="34"/>
-      <c r="B61" s="60"/>
-      <c r="C61" s="51"/>
-      <c r="D61" s="36"/>
+      <c r="A61" s="43"/>
+      <c r="B61" s="51"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="57"/>
     </row>
     <row r="62" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="34"/>
-      <c r="B62" s="60"/>
-      <c r="C62" s="52"/>
-      <c r="D62" s="37"/>
+      <c r="A62" s="43"/>
+      <c r="B62" s="51"/>
+      <c r="C62" s="41"/>
+      <c r="D62" s="58"/>
     </row>
     <row r="63" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="33" t="s">
+      <c r="A63" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="C63" s="47" t="s">
+      <c r="B63" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="C63" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="D63" s="38"/>
+      <c r="D63" s="68" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="64" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="34"/>
-      <c r="B64" s="60"/>
-      <c r="C64" s="48"/>
-      <c r="D64" s="39"/>
+      <c r="A64" s="43"/>
+      <c r="B64" s="65"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="69"/>
     </row>
     <row r="65" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A65" s="34"/>
-      <c r="B65" s="60"/>
-      <c r="C65" s="48"/>
-      <c r="D65" s="39"/>
+      <c r="A65" s="43"/>
+      <c r="B65" s="65"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="69"/>
     </row>
     <row r="66" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="34"/>
-      <c r="B66" s="60"/>
-      <c r="C66" s="49"/>
-      <c r="D66" s="40"/>
+      <c r="A66" s="43"/>
+      <c r="B66" s="65"/>
+      <c r="C66" s="38"/>
+      <c r="D66" s="70"/>
     </row>
     <row r="67" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="33" t="s">
+      <c r="A67" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="B67" s="67" t="s">
+      <c r="B67" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="C67" s="47" t="s">
+      <c r="C67" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="D67" s="64" t="s">
+      <c r="D67" s="59" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="34"/>
-      <c r="B68" s="68"/>
-      <c r="C68" s="48"/>
-      <c r="D68" s="65"/>
+      <c r="A68" s="43"/>
+      <c r="B68" s="54"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="60"/>
     </row>
     <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="34"/>
-      <c r="B69" s="68"/>
-      <c r="C69" s="48"/>
-      <c r="D69" s="65"/>
+      <c r="A69" s="43"/>
+      <c r="B69" s="54"/>
+      <c r="C69" s="37"/>
+      <c r="D69" s="60"/>
     </row>
     <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="34"/>
-      <c r="B70" s="68"/>
-      <c r="C70" s="48"/>
-      <c r="D70" s="65"/>
+      <c r="A70" s="43"/>
+      <c r="B70" s="54"/>
+      <c r="C70" s="37"/>
+      <c r="D70" s="60"/>
     </row>
     <row r="71" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="34"/>
-      <c r="B71" s="69"/>
-      <c r="C71" s="49"/>
-      <c r="D71" s="66"/>
-    </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+      <c r="A71" s="43"/>
+      <c r="B71" s="55"/>
+      <c r="C71" s="38"/>
+      <c r="D71" s="61"/>
+    </row>
+    <row r="72" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="67" t="s">
         <v>69</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C72" s="29" t="s">
+      <c r="C72" s="66" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D74" s="5"/>
+      <c r="D74" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="D59:D62"/>
+    <mergeCell ref="D67:D71"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="D53:D54"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A22:D22"/>
@@ -1836,11 +1825,6 @@
     <mergeCell ref="B59:B62"/>
     <mergeCell ref="B63:B66"/>
     <mergeCell ref="B67:B71"/>
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="D59:D62"/>
-    <mergeCell ref="D67:D71"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="D53:D54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>